<commit_message>
added data for salmon time-series and numerous updates to scripts for figures
</commit_message>
<xml_diff>
--- a/Data/1_BCSalmon.xlsx
+++ b/Data/1_BCSalmon.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leilakrichel/Desktop/GitHub/BCSalmonDisease/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3623121-9299-CC47-8D86-83A52B535687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26146C03-4048-2747-A379-F920AC9FE895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="500" windowWidth="27080" windowHeight="17500" xr2:uid="{EACFF13F-BA2D-4B47-B19F-32FC3CE0875F}"/>
+    <workbookView xWindow="660" yWindow="500" windowWidth="27080" windowHeight="17500" activeTab="1" xr2:uid="{EACFF13F-BA2D-4B47-B19F-32FC3CE0875F}"/>
   </bookViews>
   <sheets>
     <sheet name="aquaculture_production" sheetId="1" r:id="rId1"/>
     <sheet name="wild_caught" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>year</t>
   </si>
@@ -519,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E088C45F-97D5-0047-B712-E5588161AF90}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -764,7 +765,7 @@
         <v>24362</v>
       </c>
       <c r="F16">
-        <f>SUM(E16:E16)</f>
+        <f t="shared" ref="F16:F30" si="0">SUM(E16:E16)</f>
         <v>24362</v>
       </c>
       <c r="G16">
@@ -779,7 +780,7 @@
         <v>19814</v>
       </c>
       <c r="F17">
-        <f>SUM(E17:E17)</f>
+        <f t="shared" si="0"/>
         <v>19814</v>
       </c>
       <c r="G17">
@@ -794,7 +795,7 @@
         <v>25555</v>
       </c>
       <c r="F18">
-        <f>SUM(E18:E18)</f>
+        <f t="shared" si="0"/>
         <v>25555</v>
       </c>
       <c r="G18">
@@ -809,7 +810,7 @@
         <v>23657</v>
       </c>
       <c r="F19">
-        <f>SUM(E19:E19)</f>
+        <f t="shared" si="0"/>
         <v>23657</v>
       </c>
       <c r="G19">
@@ -824,7 +825,7 @@
         <v>27275</v>
       </c>
       <c r="F20">
-        <f>SUM(E20:E20)</f>
+        <f t="shared" si="0"/>
         <v>27275</v>
       </c>
       <c r="G20">
@@ -839,7 +840,7 @@
         <v>27756</v>
       </c>
       <c r="F21">
-        <f>SUM(E21:E21)</f>
+        <f t="shared" si="0"/>
         <v>27756</v>
       </c>
       <c r="G21">
@@ -854,7 +855,7 @@
         <v>36465</v>
       </c>
       <c r="F22">
-        <f>SUM(E22:E22)</f>
+        <f t="shared" si="0"/>
         <v>36465</v>
       </c>
       <c r="G22">
@@ -869,7 +870,7 @@
         <v>42200</v>
       </c>
       <c r="F23">
-        <f>SUM(E23:E23)</f>
+        <f t="shared" si="0"/>
         <v>42200</v>
       </c>
       <c r="G23">
@@ -884,7 +885,7 @@
         <v>49700</v>
       </c>
       <c r="F24">
-        <f>SUM(E24:E24)</f>
+        <f t="shared" si="0"/>
         <v>49700</v>
       </c>
       <c r="G24">
@@ -899,7 +900,7 @@
         <v>49000</v>
       </c>
       <c r="F25">
-        <f>SUM(E25:E25)</f>
+        <f t="shared" si="0"/>
         <v>49000</v>
       </c>
       <c r="G25">
@@ -914,7 +915,7 @@
         <v>68000</v>
       </c>
       <c r="F26">
-        <f>SUM(E26:E26)</f>
+        <f t="shared" si="0"/>
         <v>68000</v>
       </c>
       <c r="G26">
@@ -929,7 +930,7 @@
         <v>84200</v>
       </c>
       <c r="F27">
-        <f>SUM(E27:E27)</f>
+        <f t="shared" si="0"/>
         <v>84200</v>
       </c>
       <c r="G27">
@@ -944,7 +945,7 @@
         <v>65411</v>
       </c>
       <c r="F28">
-        <f>SUM(E28:E28)</f>
+        <f t="shared" si="0"/>
         <v>65411</v>
       </c>
       <c r="G28">
@@ -959,7 +960,7 @@
         <v>55646</v>
       </c>
       <c r="F29">
-        <f>SUM(E29:E29)</f>
+        <f t="shared" si="0"/>
         <v>55646</v>
       </c>
       <c r="G29">
@@ -974,7 +975,7 @@
         <v>63370</v>
       </c>
       <c r="F30">
-        <f>SUM(E30:E30)</f>
+        <f t="shared" si="0"/>
         <v>63370</v>
       </c>
       <c r="G30">
@@ -1003,7 +1004,7 @@
         <v>70998</v>
       </c>
       <c r="F32">
-        <f>SUM(E32:E32)</f>
+        <f t="shared" ref="F32:F37" si="1">SUM(E32:E32)</f>
         <v>70998</v>
       </c>
       <c r="G32">
@@ -1018,7 +1019,7 @@
         <v>73265</v>
       </c>
       <c r="F33">
-        <f>SUM(E33:E33)</f>
+        <f t="shared" si="1"/>
         <v>73265</v>
       </c>
       <c r="G33">
@@ -1033,7 +1034,7 @@
         <v>68662</v>
       </c>
       <c r="F34">
-        <f>SUM(E34:E34)</f>
+        <f t="shared" si="1"/>
         <v>68662</v>
       </c>
       <c r="G34">
@@ -1048,7 +1049,7 @@
         <v>70831</v>
       </c>
       <c r="F35">
-        <f>SUM(E35:E35)</f>
+        <f t="shared" si="1"/>
         <v>70831</v>
       </c>
       <c r="G35">
@@ -1063,7 +1064,7 @@
         <v>83144</v>
       </c>
       <c r="F36">
-        <f>SUM(E36:E36)</f>
+        <f t="shared" si="1"/>
         <v>83144</v>
       </c>
       <c r="G36">
@@ -1078,7 +1079,7 @@
         <v>79981</v>
       </c>
       <c r="F37">
-        <f>SUM(E37:E37)</f>
+        <f t="shared" si="1"/>
         <v>79981</v>
       </c>
       <c r="G37">
@@ -1107,7 +1108,7 @@
         <v>54971</v>
       </c>
       <c r="F39">
-        <f>SUM(E39:E39)</f>
+        <f t="shared" ref="F39:F46" si="2">SUM(E39:E39)</f>
         <v>54971</v>
       </c>
       <c r="G39">
@@ -1122,7 +1123,7 @@
         <v>92926</v>
       </c>
       <c r="F40">
-        <f>SUM(E40:E40)</f>
+        <f t="shared" si="2"/>
         <v>92926</v>
       </c>
       <c r="G40">
@@ -1137,7 +1138,7 @@
         <v>90511</v>
       </c>
       <c r="F41">
-        <f>SUM(E41:E41)</f>
+        <f t="shared" si="2"/>
         <v>90511</v>
       </c>
       <c r="G41">
@@ -1152,7 +1153,7 @@
         <v>85608</v>
       </c>
       <c r="F42">
-        <f>SUM(E42:E42)</f>
+        <f t="shared" si="2"/>
         <v>85608</v>
       </c>
       <c r="G42">
@@ -1167,7 +1168,7 @@
         <v>87010</v>
       </c>
       <c r="F43">
-        <f>SUM(E43:E43)</f>
+        <f t="shared" si="2"/>
         <v>87010</v>
       </c>
       <c r="G43">
@@ -1182,7 +1183,7 @@
         <v>88874</v>
       </c>
       <c r="F44">
-        <f>SUM(E44:E44)</f>
+        <f t="shared" si="2"/>
         <v>88874</v>
       </c>
       <c r="G44">
@@ -1197,7 +1198,7 @@
         <v>91666</v>
       </c>
       <c r="F45">
-        <f>SUM(E45:E45)</f>
+        <f t="shared" si="2"/>
         <v>91666</v>
       </c>
       <c r="G45">
@@ -1212,7 +1213,7 @@
         <v>84171</v>
       </c>
       <c r="F46">
-        <f>SUM(E46:E46)</f>
+        <f t="shared" si="2"/>
         <v>84171</v>
       </c>
       <c r="G46">
@@ -1228,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F84AE8C-9709-7A46-84C1-3053E6E69CA2}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1861,4 +1862,640 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D95669-BE80-C74C-BFB6-FF0B2D332678}">
+  <dimension ref="A1:G46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="6" width="22.33203125" customWidth="1"/>
+    <col min="7" max="7" width="28.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1977</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1978</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1979</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1980</v>
+      </c>
+      <c r="G5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1981</v>
+      </c>
+      <c r="G6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1982</v>
+      </c>
+      <c r="G7">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1983</v>
+      </c>
+      <c r="G8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1984</v>
+      </c>
+      <c r="G9">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1985</v>
+      </c>
+      <c r="G10">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1986</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>87</v>
+      </c>
+      <c r="D11">
+        <v>304</v>
+      </c>
+      <c r="G11">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1987</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>949</v>
+      </c>
+      <c r="D12">
+        <v>791</v>
+      </c>
+      <c r="G12">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1988</v>
+      </c>
+      <c r="B13">
+        <v>80</v>
+      </c>
+      <c r="C13">
+        <v>3545</v>
+      </c>
+      <c r="D13">
+        <v>2743</v>
+      </c>
+      <c r="G13">
+        <v>3431</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1989</v>
+      </c>
+      <c r="B14">
+        <v>1280</v>
+      </c>
+      <c r="C14">
+        <v>8514</v>
+      </c>
+      <c r="D14">
+        <v>1815</v>
+      </c>
+      <c r="G14">
+        <v>5967</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1990</v>
+      </c>
+      <c r="B15">
+        <v>1640</v>
+      </c>
+      <c r="C15">
+        <v>10396</v>
+      </c>
+      <c r="D15">
+        <v>1296</v>
+      </c>
+      <c r="G15">
+        <v>9625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1991</v>
+      </c>
+      <c r="E16">
+        <v>24362</v>
+      </c>
+      <c r="F16">
+        <v>34109</v>
+      </c>
+      <c r="G16">
+        <v>13499</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1992</v>
+      </c>
+      <c r="E17">
+        <v>19814</v>
+      </c>
+      <c r="F17">
+        <v>30325</v>
+      </c>
+      <c r="G17">
+        <v>17305</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1993</v>
+      </c>
+      <c r="E18">
+        <v>25555</v>
+      </c>
+      <c r="F18">
+        <v>36670</v>
+      </c>
+      <c r="G18">
+        <v>23483</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1994</v>
+      </c>
+      <c r="E19">
+        <v>23657</v>
+      </c>
+      <c r="F19">
+        <v>23657</v>
+      </c>
+      <c r="G19">
+        <v>27773</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1995</v>
+      </c>
+      <c r="E20">
+        <v>27275</v>
+      </c>
+      <c r="F20">
+        <v>42515</v>
+      </c>
+      <c r="G20">
+        <v>33674</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1996</v>
+      </c>
+      <c r="E21">
+        <v>27756</v>
+      </c>
+      <c r="F21">
+        <v>45624</v>
+      </c>
+      <c r="G21">
+        <v>36475</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1997</v>
+      </c>
+      <c r="E22">
+        <v>36465</v>
+      </c>
+      <c r="F22">
+        <v>56775</v>
+      </c>
+      <c r="G22">
+        <v>51015</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1998</v>
+      </c>
+      <c r="E23">
+        <v>42200</v>
+      </c>
+      <c r="F23">
+        <v>58618</v>
+      </c>
+      <c r="G23">
+        <v>49475</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1999</v>
+      </c>
+      <c r="E24">
+        <v>49700</v>
+      </c>
+      <c r="F24">
+        <v>72890</v>
+      </c>
+      <c r="G24">
+        <v>61990</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2000</v>
+      </c>
+      <c r="E25">
+        <v>49000</v>
+      </c>
+      <c r="F25">
+        <v>82195</v>
+      </c>
+      <c r="G25">
+        <v>72495</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2001</v>
+      </c>
+      <c r="E26">
+        <v>68000</v>
+      </c>
+      <c r="F26">
+        <v>105606</v>
+      </c>
+      <c r="G26">
+        <v>95606</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2002</v>
+      </c>
+      <c r="E27">
+        <v>84200</v>
+      </c>
+      <c r="F27">
+        <v>126321</v>
+      </c>
+      <c r="G27">
+        <v>114921</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2003</v>
+      </c>
+      <c r="E28">
+        <v>65411</v>
+      </c>
+      <c r="F28">
+        <v>99961</v>
+      </c>
+      <c r="G28">
+        <v>107228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2004</v>
+      </c>
+      <c r="E29">
+        <v>55646</v>
+      </c>
+      <c r="F29">
+        <v>90646</v>
+      </c>
+      <c r="G29">
+        <v>96774</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2005</v>
+      </c>
+      <c r="E30">
+        <v>63370</v>
+      </c>
+      <c r="F30">
+        <v>98370</v>
+      </c>
+      <c r="G30">
+        <v>98370</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2006</v>
+      </c>
+      <c r="E31">
+        <v>70181</v>
+      </c>
+      <c r="F31" s="1">
+        <v>118061</v>
+      </c>
+      <c r="G31">
+        <v>118061</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2007</v>
+      </c>
+      <c r="E32">
+        <v>70998</v>
+      </c>
+      <c r="F32">
+        <v>102509</v>
+      </c>
+      <c r="G32">
+        <v>102509</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2008</v>
+      </c>
+      <c r="E33">
+        <v>73265</v>
+      </c>
+      <c r="F33">
+        <v>104075</v>
+      </c>
+      <c r="G33">
+        <v>104075</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2009</v>
+      </c>
+      <c r="E34">
+        <v>68662</v>
+      </c>
+      <c r="F34">
+        <v>100212</v>
+      </c>
+      <c r="G34">
+        <v>100212</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2010</v>
+      </c>
+      <c r="E35">
+        <v>70831</v>
+      </c>
+      <c r="F35">
+        <v>101544</v>
+      </c>
+      <c r="G35">
+        <v>101544</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2011</v>
+      </c>
+      <c r="E36">
+        <v>83144</v>
+      </c>
+      <c r="F36">
+        <v>110328</v>
+      </c>
+      <c r="G36">
+        <v>110328</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2012</v>
+      </c>
+      <c r="E37">
+        <v>79981</v>
+      </c>
+      <c r="F37">
+        <v>116101</v>
+      </c>
+      <c r="G37">
+        <v>116101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2013</v>
+      </c>
+      <c r="E38">
+        <v>74673</v>
+      </c>
+      <c r="F38">
+        <v>100027</v>
+      </c>
+      <c r="G38">
+        <v>97629</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2014</v>
+      </c>
+      <c r="E39">
+        <v>54971</v>
+      </c>
+      <c r="F39">
+        <v>78979</v>
+      </c>
+      <c r="G39">
+        <v>86347</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2015</v>
+      </c>
+      <c r="E40">
+        <v>92926</v>
+      </c>
+      <c r="F40">
+        <v>121926</v>
+      </c>
+      <c r="G40">
+        <v>121926</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2016</v>
+      </c>
+      <c r="E41">
+        <v>90511</v>
+      </c>
+      <c r="F41">
+        <v>123522</v>
+      </c>
+      <c r="G41">
+        <v>123522</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2017</v>
+      </c>
+      <c r="E42">
+        <v>85608</v>
+      </c>
+      <c r="F42">
+        <v>120553</v>
+      </c>
+      <c r="G42">
+        <v>120553</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2018</v>
+      </c>
+      <c r="E43">
+        <v>87010</v>
+      </c>
+      <c r="F43">
+        <v>123184</v>
+      </c>
+      <c r="G43">
+        <v>123184</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2019</v>
+      </c>
+      <c r="E44">
+        <v>88874</v>
+      </c>
+      <c r="F44">
+        <v>118632</v>
+      </c>
+      <c r="G44">
+        <v>118630</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2020</v>
+      </c>
+      <c r="E45">
+        <v>91666</v>
+      </c>
+      <c r="F45">
+        <v>120285</v>
+      </c>
+      <c r="G45">
+        <v>120427</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2021</v>
+      </c>
+      <c r="E46">
+        <v>84171</v>
+      </c>
+      <c r="F46">
+        <v>120186</v>
+      </c>
+      <c r="G46">
+        <v>120186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>